<commit_message>
Mass Budget and Mars
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armaa\Desktop\I2S\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakima Lakhder\Documents\GitHub\Intro2Spaceflight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA73E14-24F6-45AC-9C9D-9B76B3D2243F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5312F485-397B-4EC8-AA6E-BEDCB8635C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="2" r:id="rId1"/>
@@ -159,7 +159,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -474,14 +474,14 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11.26953125" customWidth="1"/>
-    <col min="3" max="3" width="5.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -529,35 +529,35 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>-8035822.75</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>22289</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>290</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -684,5 +684,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>